<commit_message>
Fix: Correction double-encodage UTF-8 des noms IRIS (Épine, à, etc.)
</commit_message>
<xml_diff>
--- a/DATASET scores brut.xlsx
+++ b/DATASET scores brut.xlsx
@@ -1719,7 +1719,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Ãpine Mont de Terre 1</t>
+          <t>Épine Mont de Terre 1</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -1813,7 +1813,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Ãpine Mont de Terre 5</t>
+          <t>Épine Mont de Terre 5</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -8863,7 +8863,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Ãpine Mont de Terre 2</t>
+          <t>Épine Mont de Terre 2</t>
         </is>
       </c>
       <c r="C90" t="n">
@@ -8957,7 +8957,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Ãpine Mont de Terre 3</t>
+          <t>Épine Mont de Terre 3</t>
         </is>
       </c>
       <c r="C91" t="n">
@@ -9051,7 +9051,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Ãpine Mont de Terre 4</t>
+          <t>Épine Mont de Terre 4</t>
         </is>
       </c>
       <c r="C92" t="n">
@@ -10273,7 +10273,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Mont Ã  Camp-Marais 1</t>
+          <t>Mont à Camp-Marais 1</t>
         </is>
       </c>
       <c r="C105" t="n">
@@ -10367,7 +10367,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Mont Ã  Camp-Marais 2</t>
+          <t>Mont à Camp-Marais 2</t>
         </is>
       </c>
       <c r="C106" t="n">
@@ -10461,7 +10461,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Mont Ã  Camp-Marais 3</t>
+          <t>Mont à Camp-Marais 3</t>
         </is>
       </c>
       <c r="C107" t="n">
@@ -10555,7 +10555,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Mont Ã  Camp-Marais 4</t>
+          <t>Mont à Camp-Marais 4</t>
         </is>
       </c>
       <c r="C108" t="n">

</xml_diff>